<commit_message>
checkpoint returned good result over 50 days
</commit_message>
<xml_diff>
--- a/listOfStocks.xlsx
+++ b/listOfStocks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>CTIC</t>
   </si>
@@ -552,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -584,7 +584,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
@@ -671,87 +671,87 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:1">
@@ -761,90 +761,58 @@
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:A46">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>